<commit_message>
Normalization of the table in Dystrybucja database
</commit_message>
<xml_diff>
--- a/Dystrybucja.xlsx
+++ b/Dystrybucja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubah\Desktop\AGH zajecia\Bazy danych laborki\Cwiczenia_7a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0513C18F-3577-4794-8B5E-194CFE0DEB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48D018E-50BA-4181-91AD-6A9AFB13CF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="0" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>IDProduktu</t>
   </si>
@@ -264,6 +264,21 @@
   </si>
   <si>
     <t>C3</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
   </si>
 </sst>
 </file>
@@ -271,7 +286,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;zł&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -553,13 +568,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -860,7 +875,7 @@
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,8 +962,8 @@
       <c r="M4" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="8">
-        <v>1</v>
+      <c r="N4" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
@@ -974,8 +989,8 @@
       <c r="M5" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="8">
-        <v>2</v>
+      <c r="N5" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1001,8 +1016,8 @@
       <c r="M6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="8">
-        <v>3</v>
+      <c r="N6" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -1012,8 +1027,8 @@
       <c r="M7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="8">
-        <v>4</v>
+      <c r="N7" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1023,8 +1038,8 @@
       <c r="M8" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="N8" s="10">
-        <v>5</v>
+      <c r="N8" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1069,8 +1084,8 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="22">
-        <v>1</v>
+      <c r="B12" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>33</v>
@@ -1092,8 +1107,8 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="22">
-        <v>2</v>
+      <c r="B13" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>34</v>
@@ -1115,8 +1130,8 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="22">
-        <v>3</v>
+      <c r="B14" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>36</v>
@@ -1138,8 +1153,8 @@
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="22">
-        <v>4</v>
+      <c r="B15" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>38</v>
@@ -1161,8 +1176,8 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="25">
-        <v>5</v>
+      <c r="B16" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="C16" s="29" t="s">
         <v>39</v>

</xml_diff>